<commit_message>
Add new way of automation
</commit_message>
<xml_diff>
--- a/instagram.xlsx
+++ b/instagram.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="425">
   <si>
     <t>_vikranth_shetty_</t>
   </si>
@@ -677,6 +677,618 @@
   </si>
   <si>
     <t>notmannat</t>
+  </si>
+  <si>
+    <t>maria.onthemove</t>
+  </si>
+  <si>
+    <t>hwajess_55</t>
+  </si>
+  <si>
+    <t>meem.qtr___</t>
+  </si>
+  <si>
+    <t>its._only</t>
+  </si>
+  <si>
+    <t>fxwxe</t>
+  </si>
+  <si>
+    <t>ataag_</t>
+  </si>
+  <si>
+    <t>vjg1h</t>
+  </si>
+  <si>
+    <t>mmanoory__</t>
+  </si>
+  <si>
+    <t>00l0x</t>
+  </si>
+  <si>
+    <t>samaralmaidany</t>
+  </si>
+  <si>
+    <t>sh300l11</t>
+  </si>
+  <si>
+    <t>__g0697</t>
+  </si>
+  <si>
+    <t>abi_alnasr</t>
+  </si>
+  <si>
+    <t>mnayer000</t>
+  </si>
+  <si>
+    <t>phillip_rafco</t>
+  </si>
+  <si>
+    <t>roula_zuhair</t>
+  </si>
+  <si>
+    <t>_sairasif_</t>
+  </si>
+  <si>
+    <t>pallanmark</t>
+  </si>
+  <si>
+    <t>maha.a.almana</t>
+  </si>
+  <si>
+    <t>awadallah.hadeel</t>
+  </si>
+  <si>
+    <t>q_gs_q</t>
+  </si>
+  <si>
+    <t>premio.lb</t>
+  </si>
+  <si>
+    <t>malthanii</t>
+  </si>
+  <si>
+    <t>shamamahhhhhhh</t>
+  </si>
+  <si>
+    <t>has0osi</t>
+  </si>
+  <si>
+    <t>nbf1_</t>
+  </si>
+  <si>
+    <t>whateverj882</t>
+  </si>
+  <si>
+    <t>deeena_ahmad7</t>
+  </si>
+  <si>
+    <t>aliqatar9900</t>
+  </si>
+  <si>
+    <t>burakkilavuz</t>
+  </si>
+  <si>
+    <t>abeermarmash</t>
+  </si>
+  <si>
+    <t>xh270</t>
+  </si>
+  <si>
+    <t>a_b_333</t>
+  </si>
+  <si>
+    <t>ma_ha7164</t>
+  </si>
+  <si>
+    <t>yyba89</t>
+  </si>
+  <si>
+    <t>m86gomaa</t>
+  </si>
+  <si>
+    <t>mbm_81</t>
+  </si>
+  <si>
+    <t>yasmine_wohoosh</t>
+  </si>
+  <si>
+    <t>ajmal.sayyed</t>
+  </si>
+  <si>
+    <t>a212ali</t>
+  </si>
+  <si>
+    <t>alkubaisin11</t>
+  </si>
+  <si>
+    <t>a__1100__</t>
+  </si>
+  <si>
+    <t>dalal_almosallam</t>
+  </si>
+  <si>
+    <t>marwa_albukhari</t>
+  </si>
+  <si>
+    <t>nkammourah</t>
+  </si>
+  <si>
+    <t>xtbm8</t>
+  </si>
+  <si>
+    <t>abe93__</t>
+  </si>
+  <si>
+    <t>t1nhn</t>
+  </si>
+  <si>
+    <t>laadydiary</t>
+  </si>
+  <si>
+    <t>ha_19933</t>
+  </si>
+  <si>
+    <t>elena_kanello</t>
+  </si>
+  <si>
+    <t>fadila.6</t>
+  </si>
+  <si>
+    <t>nbiiintm</t>
+  </si>
+  <si>
+    <t>mvneer.a</t>
+  </si>
+  <si>
+    <t>de.almannaii</t>
+  </si>
+  <si>
+    <t>delizioso.qa</t>
+  </si>
+  <si>
+    <t>aeyy66</t>
+  </si>
+  <si>
+    <t>shop_qatar974</t>
+  </si>
+  <si>
+    <t>h110</t>
+  </si>
+  <si>
+    <t>azznaj</t>
+  </si>
+  <si>
+    <t>91_mba</t>
+  </si>
+  <si>
+    <t>j_ni</t>
+  </si>
+  <si>
+    <t>nadejdaay</t>
+  </si>
+  <si>
+    <t>3bood_dave</t>
+  </si>
+  <si>
+    <t>memo_senorita</t>
+  </si>
+  <si>
+    <t>alajmiabdullah422</t>
+  </si>
+  <si>
+    <t>mashail_al_mtairy9</t>
+  </si>
+  <si>
+    <t>h_al3bdulla</t>
+  </si>
+  <si>
+    <t>_.ran10</t>
+  </si>
+  <si>
+    <t>3li_q3</t>
+  </si>
+  <si>
+    <t>loyalty_qtr</t>
+  </si>
+  <si>
+    <t>u0shy</t>
+  </si>
+  <si>
+    <t>ahmad.m.08</t>
+  </si>
+  <si>
+    <t>labintm</t>
+  </si>
+  <si>
+    <t>haneen5184</t>
+  </si>
+  <si>
+    <t>alhumaidimohammed123</t>
+  </si>
+  <si>
+    <t>_m6dp</t>
+  </si>
+  <si>
+    <t>qtr907466</t>
+  </si>
+  <si>
+    <t>lama5050</t>
+  </si>
+  <si>
+    <t>ga.1811</t>
+  </si>
+  <si>
+    <t>almarr2</t>
+  </si>
+  <si>
+    <t>amera__almarri__</t>
+  </si>
+  <si>
+    <t>rouwaida_flayfel</t>
+  </si>
+  <si>
+    <t>saraknio</t>
+  </si>
+  <si>
+    <t>jx.qtri</t>
+  </si>
+  <si>
+    <t>alotaiibii2_</t>
+  </si>
+  <si>
+    <t>izzzd_</t>
+  </si>
+  <si>
+    <t>mmn3060</t>
+  </si>
+  <si>
+    <t>imixq</t>
+  </si>
+  <si>
+    <t>amooona1983</t>
+  </si>
+  <si>
+    <t>sandra1462015</t>
+  </si>
+  <si>
+    <t>__soso_00</t>
+  </si>
+  <si>
+    <t>09sep_</t>
+  </si>
+  <si>
+    <t>blue_lagoon_spa</t>
+  </si>
+  <si>
+    <t>rkr.10</t>
+  </si>
+  <si>
+    <t>afa.althanii</t>
+  </si>
+  <si>
+    <t>x.m.91.x</t>
+  </si>
+  <si>
+    <t>qtrimem</t>
+  </si>
+  <si>
+    <t>lattiqat</t>
+  </si>
+  <si>
+    <t>mbiomy</t>
+  </si>
+  <si>
+    <t>aishaa.9x</t>
+  </si>
+  <si>
+    <t>soso_events</t>
+  </si>
+  <si>
+    <t>phosphenes_qatar</t>
+  </si>
+  <si>
+    <t>faisal_almehshadi</t>
+  </si>
+  <si>
+    <t>shintojoseph777</t>
+  </si>
+  <si>
+    <t>lmeybs</t>
+  </si>
+  <si>
+    <t>mba.888</t>
+  </si>
+  <si>
+    <t>s71y</t>
+  </si>
+  <si>
+    <t>m__6__1</t>
+  </si>
+  <si>
+    <t>_rawanadil</t>
+  </si>
+  <si>
+    <t>j9xd</t>
+  </si>
+  <si>
+    <t>hamasaki_1990</t>
+  </si>
+  <si>
+    <t>24.11.96_</t>
+  </si>
+  <si>
+    <t>nss__1991</t>
+  </si>
+  <si>
+    <t>wyi2l</t>
+  </si>
+  <si>
+    <t>fo0oz2012</t>
+  </si>
+  <si>
+    <t>lolo4033</t>
+  </si>
+  <si>
+    <t>ghalya.alobaidly</t>
+  </si>
+  <si>
+    <t>burger_showqtr</t>
+  </si>
+  <si>
+    <t>mralfaisall</t>
+  </si>
+  <si>
+    <t>mm.m812</t>
+  </si>
+  <si>
+    <t>ercanaykan7</t>
+  </si>
+  <si>
+    <t>_i3bj</t>
+  </si>
+  <si>
+    <t>meryemguaid2019</t>
+  </si>
+  <si>
+    <t>_qxbl</t>
+  </si>
+  <si>
+    <t>glassjaronsale</t>
+  </si>
+  <si>
+    <t>makeupabeer_qtr9</t>
+  </si>
+  <si>
+    <t>aiiishaaa5</t>
+  </si>
+  <si>
+    <t>ads.qatar</t>
+  </si>
+  <si>
+    <t>totah_75_</t>
+  </si>
+  <si>
+    <t>ewan_alhajri2</t>
+  </si>
+  <si>
+    <t>x.0096</t>
+  </si>
+  <si>
+    <t>0b6__</t>
+  </si>
+  <si>
+    <t>mbxre</t>
+  </si>
+  <si>
+    <t>shmookal3az</t>
+  </si>
+  <si>
+    <t>lozan.rr</t>
+  </si>
+  <si>
+    <t>e1002xx</t>
+  </si>
+  <si>
+    <t>etoo87</t>
+  </si>
+  <si>
+    <t>tmald_</t>
+  </si>
+  <si>
+    <t>5.6f3</t>
+  </si>
+  <si>
+    <t>maryamkhan7629</t>
+  </si>
+  <si>
+    <t>jiggsylog</t>
+  </si>
+  <si>
+    <t>tathkaralhamad_</t>
+  </si>
+  <si>
+    <t>kelvincee911</t>
+  </si>
+  <si>
+    <t>noura_albuenain</t>
+  </si>
+  <si>
+    <t>almahaalkuwari94</t>
+  </si>
+  <si>
+    <t>saraahkhoja</t>
+  </si>
+  <si>
+    <t>bo_mohammad2121</t>
+  </si>
+  <si>
+    <t>_90h7</t>
+  </si>
+  <si>
+    <t>fooz___qtr</t>
+  </si>
+  <si>
+    <t>matra.alahmed</t>
+  </si>
+  <si>
+    <t>n_s_qtr11</t>
+  </si>
+  <si>
+    <t>maialkuwari</t>
+  </si>
+  <si>
+    <t>afshan1010</t>
+  </si>
+  <si>
+    <t>healthybody_sonia4</t>
+  </si>
+  <si>
+    <t>jurida_doko</t>
+  </si>
+  <si>
+    <t>pergosa.tr</t>
+  </si>
+  <si>
+    <t>ma95__q</t>
+  </si>
+  <si>
+    <t>hustohqatar</t>
+  </si>
+  <si>
+    <t>8llhy</t>
+  </si>
+  <si>
+    <t>amelcommunication007</t>
+  </si>
+  <si>
+    <t>joyaksjoyaks</t>
+  </si>
+  <si>
+    <t>1mqr</t>
+  </si>
+  <si>
+    <t>chelseabridge.qa</t>
+  </si>
+  <si>
+    <t>znsour</t>
+  </si>
+  <si>
+    <t>masviyy</t>
+  </si>
+  <si>
+    <t>arfaoui_hajer</t>
+  </si>
+  <si>
+    <t>wmatouk</t>
+  </si>
+  <si>
+    <t>mohannadnaim</t>
+  </si>
+  <si>
+    <t>qata_202020</t>
+  </si>
+  <si>
+    <t>mojarrdi.81</t>
+  </si>
+  <si>
+    <t>aiijx21</t>
+  </si>
+  <si>
+    <t>_maalmaadeed</t>
+  </si>
+  <si>
+    <t>ixxsy</t>
+  </si>
+  <si>
+    <t>ialmari_</t>
+  </si>
+  <si>
+    <t>elitebreezeltd</t>
+  </si>
+  <si>
+    <t>nvxk_</t>
+  </si>
+  <si>
+    <t>fbintalb9</t>
+  </si>
+  <si>
+    <t>shan.sampath</t>
+  </si>
+  <si>
+    <t>i7uii_</t>
+  </si>
+  <si>
+    <t>_budouralturki</t>
+  </si>
+  <si>
+    <t>j.vxyy</t>
+  </si>
+  <si>
+    <t>se_1001</t>
+  </si>
+  <si>
+    <t>sama.qtr87</t>
+  </si>
+  <si>
+    <t>alreem930124003</t>
+  </si>
+  <si>
+    <t>umslman8227</t>
+  </si>
+  <si>
+    <t>vlez18</t>
+  </si>
+  <si>
+    <t>hamada_cherkaoui_sellami</t>
+  </si>
+  <si>
+    <t>iix.aey01</t>
+  </si>
+  <si>
+    <t>kaak23kaak</t>
+  </si>
+  <si>
+    <t>ab0902_</t>
+  </si>
+  <si>
+    <t>rix_o0</t>
+  </si>
+  <si>
+    <t>salq88__</t>
+  </si>
+  <si>
+    <t>jabal7182</t>
+  </si>
+  <si>
+    <t>khulood85</t>
+  </si>
+  <si>
+    <t>ifoay</t>
+  </si>
+  <si>
+    <t>ikram_guerfala</t>
+  </si>
+  <si>
+    <t>photo_lovers9</t>
+  </si>
+  <si>
+    <t>aishalthani</t>
+  </si>
+  <si>
+    <t>q_7_q_</t>
+  </si>
+  <si>
+    <t>novalmarrri</t>
+  </si>
+  <si>
+    <t>singhshivendra18</t>
+  </si>
+  <si>
+    <t>saratmahmoud</t>
+  </si>
+  <si>
+    <t>saracabral27</t>
   </si>
 </sst>
 </file>
@@ -1013,10 +1625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A228"/>
+  <dimension ref="A1:A432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="A223" sqref="A223:A228"/>
+    <sheetView tabSelected="1" topLeftCell="A357" workbookViewId="0">
+      <selection activeCell="A229" sqref="A229:A432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2156,6 +2768,1026 @@
         <v>75</v>
       </c>
     </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>424</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>